<commit_message>
Fiddle w/ results sheet formatting
</commit_message>
<xml_diff>
--- a/results/refit-model-summary-for-Tony.xlsx
+++ b/results/refit-model-summary-for-Tony.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{073CB452-FF8F-1042-8DA8-C5585E2E3FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08E0EC6-D81F-2849-B751-7CCD9B96726B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="17040"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refit-model-summary-for-Tony" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20">
     <font>
       <sz val="12"/>
@@ -627,9 +627,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -638,6 +635,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -992,11 +992,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1015,15 +1015,15 @@
       <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D4">
@@ -1063,7 +1063,7 @@
       <c r="G4">
         <v>282.363</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I4" t="s">
@@ -1089,7 +1089,7 @@
       <c r="G5">
         <v>63.076000000000001</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I5" t="s">
@@ -1115,7 +1115,7 @@
       <c r="G6">
         <v>125.01</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I6" t="s">
@@ -1141,7 +1141,7 @@
       <c r="G7">
         <v>39.618000000000002</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I7" t="s">
@@ -1167,7 +1167,7 @@
       <c r="G8">
         <v>186.21700000000001</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I8" t="s">
@@ -1193,7 +1193,7 @@
       <c r="G9">
         <v>53.265000000000001</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>0.13800000000000001</v>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
       <c r="G10">
         <v>88.704999999999998</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I10" t="s">
@@ -1242,7 +1242,7 @@
       <c r="G11">
         <v>4.1210000000000004</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="I11" t="s">
@@ -1268,7 +1268,7 @@
       <c r="G12">
         <v>26.971</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>0.80300000000000005</v>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       <c r="G13">
         <v>82.352999999999994</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I13" t="s">
@@ -1317,12 +1317,12 @@
       <c r="G14">
         <v>23.959</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>0.77100000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="H15" s="3"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
@@ -1331,7 +1331,7 @@
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D16">
@@ -1346,7 +1346,7 @@
       <c r="G16">
         <v>896.48400000000004</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I16" t="s">
@@ -1372,7 +1372,7 @@
       <c r="G17">
         <v>198.19499999999999</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>1E-3</v>
       </c>
       <c r="I17" t="s">
@@ -1398,7 +1398,7 @@
       <c r="G18">
         <v>151.17099999999999</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="I18" t="s">
@@ -1424,7 +1424,7 @@
       <c r="G19">
         <v>366.98700000000002</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="I19" t="s">
@@ -1450,7 +1450,7 @@
       <c r="G20">
         <v>139.161</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>0.97099999999999997</v>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
       <c r="G21">
         <v>241.58</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>1.9E-2</v>
       </c>
       <c r="I21" t="s">
@@ -1499,7 +1499,7 @@
       <c r="G22">
         <v>440.28399999999999</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>1E-3</v>
       </c>
       <c r="I22" t="s">
@@ -1525,10 +1525,10 @@
       <c r="G23">
         <v>202.21799999999999</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       <c r="G24">
         <v>154.83600000000001</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>0.90100000000000002</v>
       </c>
     </row>
@@ -1574,10 +1574,10 @@
       <c r="G25">
         <v>244.90700000000001</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1600,7 +1600,7 @@
       <c r="G26">
         <v>190.18799999999999</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>0.31</v>
       </c>
     </row>
@@ -1623,10 +1623,10 @@
       <c r="G27">
         <v>15.484999999999999</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1649,7 +1649,7 @@
       <c r="G28">
         <v>11.843</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>2.3E-2</v>
       </c>
       <c r="I28" t="s">
@@ -1675,12 +1675,12 @@
       <c r="G29">
         <v>110.164</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>0.70399999999999996</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="H30" s="3"/>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
@@ -1689,7 +1689,7 @@
       <c r="B31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D31">
@@ -1704,7 +1704,7 @@
       <c r="G31">
         <v>3808.2510000000002</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I31" t="s">
@@ -1730,10 +1730,10 @@
       <c r="G32">
         <v>785.22</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1756,7 +1756,7 @@
       <c r="G33">
         <v>122.04300000000001</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="I33" t="s">
@@ -1782,7 +1782,7 @@
       <c r="G34">
         <v>62.814</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="I34" t="s">
@@ -1808,7 +1808,7 @@
       <c r="G35">
         <v>-667.596</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I35" t="s">
@@ -1834,7 +1834,7 @@
       <c r="G36">
         <v>-1099.6600000000001</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I36" t="s">
@@ -1860,7 +1860,7 @@
       <c r="G37">
         <v>405.28100000000001</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="2">
         <v>0.219</v>
       </c>
     </row>
@@ -1883,7 +1883,7 @@
       <c r="G38">
         <v>853.11300000000006</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I38" t="s">
@@ -1909,7 +1909,7 @@
       <c r="G39">
         <v>582.02300000000002</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="2">
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="I39" t="s">
@@ -1935,7 +1935,7 @@
       <c r="G40">
         <v>1231.537</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I40" t="s">
@@ -1961,7 +1961,7 @@
       <c r="G41">
         <v>410.86</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
         <v>0.68</v>
       </c>
     </row>
@@ -1984,7 +1984,7 @@
       <c r="G42">
         <v>448.91899999999998</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
         <v>0.124</v>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       <c r="G43">
         <v>257.76799999999997</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
         <v>0.68899999999999995</v>
       </c>
     </row>
@@ -2030,7 +2030,7 @@
       <c r="G44">
         <v>1556.248</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I44" t="s">
@@ -2056,10 +2056,10 @@
       <c r="G45">
         <v>508.26799999999997</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="2">
         <v>2E-3</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2082,10 +2082,10 @@
       <c r="G46">
         <v>-106.029</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="2">
         <v>2E-3</v>
       </c>
-      <c r="I46" s="5" t="s">
+      <c r="I46" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2108,7 +2108,7 @@
       <c r="G47">
         <v>192.791</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="2">
         <v>0.625</v>
       </c>
     </row>

</xml_diff>